<commit_message>
Looking at how Alts match patterns
</commit_message>
<xml_diff>
--- a/CH-145 Length of Pattern.xlsx
+++ b/CH-145 Length of Pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC3688-31EC-409D-8A70-F57651A52EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9E6AA-5101-42C6-8814-85A0249285FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="43">
   <si>
     <t>Question</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>This approach creates all the possible sequences. It then looks for those.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3333750" cy="2638425"/>
+    <xdr:ext cx="3333750" cy="2847975"/>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="2" name="Shape 2" title="Drawing">
@@ -596,9 +599,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="2293620" y="1183005"/>
-          <a:ext cx="3333750" cy="2638425"/>
+          <a:ext cx="3333750" cy="2847975"/>
           <a:chOff x="3688650" y="2470313"/>
-          <a:chExt cx="3314700" cy="2619375"/>
+          <a:chExt cx="3314700" cy="2827412"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -615,9 +618,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="3688650" y="2470313"/>
-            <a:ext cx="3314700" cy="2619375"/>
+            <a:ext cx="3314700" cy="2827412"/>
             <a:chOff x="2286664" y="1181098"/>
-            <a:chExt cx="3342611" cy="2581277"/>
+            <a:chExt cx="3342611" cy="2786288"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -773,7 +776,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="2733675" y="1501775"/>
-              <a:ext cx="2895600" cy="2260600"/>
+              <a:ext cx="2895600" cy="2465611"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst>
@@ -1592,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -8086,8 +8089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6FED8D-D1B5-4F6C-A9EF-769F17A8CA37}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -14606,7 +14609,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -14886,6 +14889,9 @@
         <v>12</v>
       </c>
       <c r="E8" s="10"/>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -21120,7 +21126,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Breaking down the REGEX
</commit_message>
<xml_diff>
--- a/CH-145 Length of Pattern.xlsx
+++ b/CH-145 Length of Pattern.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9E6AA-5101-42C6-8814-85A0249285FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C5174-669B-469B-9D5A-AB59E693D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="44">
   <si>
     <t>Question</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>This approach creates all the possible sequences. It then looks for those.</t>
+  </si>
+  <si>
+    <t>This is clever. Use GROUPBY to pick up all the sequential letters.</t>
   </si>
 </sst>
 </file>
@@ -8089,8 +8092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6FED8D-D1B5-4F6C-A9EF-769F17A8CA37}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -8370,6 +8373,9 @@
         <v>12</v>
       </c>
       <c r="E8" s="10"/>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -14608,7 +14614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98ED4F9-8303-4125-B6A5-1B4E53352205}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I am now seeing how the REGEX works
</commit_message>
<xml_diff>
--- a/CH-145 Length of Pattern.xlsx
+++ b/CH-145 Length of Pattern.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C5174-669B-469B-9D5A-AB59E693D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517BA47-92C2-4071-A47E-082C30175AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1598,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -8092,8 +8092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6FED8D-D1B5-4F6C-A9EF-769F17A8CA37}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -8450,10 +8450,18 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="2" t="str" cm="1">
+        <f t="array" ref="N10:O19">_xlfn._xlws.FILTER(C3:D32,C3:C32="B")</f>
+        <v>B</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <v>-</v>
+      </c>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="Q10" s="2" t="str" cm="1">
+        <f t="array" ref="Q10">_xlfn.LET(_xlpm.x, O10:O19,_xlfn.REGEXEXTRACT(_xlfn.CONCAT(_xlpm.x), "(\+\+-)+(\+\+?)?"))</f>
+        <v>++-++-+</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -8485,8 +8493,12 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="N11" s="2" t="str">
+        <v>B</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <v>+</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -8520,8 +8532,12 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="N12" s="2" t="str">
+        <v>B</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <v>+</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -8545,6 +8561,12 @@
         <v>12</v>
       </c>
       <c r="E13" s="13"/>
+      <c r="N13" t="str">
+        <v>B</v>
+      </c>
+      <c r="O13" t="str">
+        <v>+</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1">
       <c r="B14" s="8" t="s">
@@ -8557,6 +8579,12 @@
         <v>8</v>
       </c>
       <c r="E14" s="13"/>
+      <c r="N14" t="str">
+        <v>B</v>
+      </c>
+      <c r="O14" t="str">
+        <v>-</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="14"/>
@@ -8571,6 +8599,12 @@
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="15"/>
+      <c r="N15" t="str">
+        <v>B</v>
+      </c>
+      <c r="O15" t="str">
+        <v>+</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
       <c r="A16" s="14"/>
@@ -8585,8 +8619,14 @@
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1">
+      <c r="N16" t="str">
+        <v>B</v>
+      </c>
+      <c r="O16" t="str">
+        <v>+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="17.25" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>25</v>
@@ -8599,8 +8639,14 @@
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="17.25" customHeight="1">
+      <c r="N17" t="str">
+        <v>B</v>
+      </c>
+      <c r="O17" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17.25" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
         <v>26</v>
@@ -8613,8 +8659,14 @@
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1">
+      <c r="N18" t="str">
+        <v>B</v>
+      </c>
+      <c r="O18" t="str">
+        <v>+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="17.25" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>27</v>
@@ -8627,8 +8679,14 @@
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" customHeight="1">
+      <c r="N19" t="str">
+        <v>B</v>
+      </c>
+      <c r="O19" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="17.25" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>28</v>
@@ -8642,7 +8700,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" ht="17.25" customHeight="1">
+    <row r="21" spans="1:15" ht="17.25" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -8656,7 +8714,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" ht="17.25" customHeight="1">
+    <row r="22" spans="1:15" ht="17.25" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="8" t="s">
         <v>30</v>
@@ -8670,7 +8728,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" ht="17.25" customHeight="1">
+    <row r="23" spans="1:15" ht="17.25" customHeight="1">
       <c r="B23" s="8" t="s">
         <v>31</v>
       </c>
@@ -8683,7 +8741,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" ht="17.25" customHeight="1">
+    <row r="24" spans="1:15" ht="17.25" customHeight="1">
       <c r="B24" s="8" t="s">
         <v>32</v>
       </c>
@@ -8695,7 +8753,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" ht="17.25" customHeight="1">
+    <row r="25" spans="1:15" ht="17.25" customHeight="1">
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
@@ -8707,7 +8765,7 @@
       </c>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" spans="1:6" ht="17.25" customHeight="1">
+    <row r="26" spans="1:15" ht="17.25" customHeight="1">
       <c r="B26" s="8" t="s">
         <v>34</v>
       </c>
@@ -8719,7 +8777,7 @@
       </c>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" ht="17.25" customHeight="1">
+    <row r="27" spans="1:15" ht="17.25" customHeight="1">
       <c r="B27" s="8" t="s">
         <v>35</v>
       </c>
@@ -8731,7 +8789,7 @@
       </c>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" ht="17.25" customHeight="1">
+    <row r="28" spans="1:15" ht="17.25" customHeight="1">
       <c r="B28" s="8" t="s">
         <v>36</v>
       </c>
@@ -8743,7 +8801,7 @@
       </c>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" ht="17.25" customHeight="1">
+    <row r="29" spans="1:15" ht="17.25" customHeight="1">
       <c r="B29" s="8" t="s">
         <v>37</v>
       </c>
@@ -8755,7 +8813,7 @@
       </c>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="17.25" customHeight="1">
+    <row r="30" spans="1:15" ht="17.25" customHeight="1">
       <c r="B30" s="8" t="s">
         <v>38</v>
       </c>
@@ -8767,7 +8825,7 @@
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" ht="17.25" customHeight="1">
+    <row r="31" spans="1:15" ht="17.25" customHeight="1">
       <c r="B31" s="8" t="s">
         <v>39</v>
       </c>
@@ -8779,7 +8837,7 @@
       </c>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" spans="1:6" ht="17.25" customHeight="1">
+    <row r="32" spans="1:15" ht="17.25" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>40</v>
       </c>

</xml_diff>